<commit_message>
Fixed binomial glms and added analysis on qPCR
</commit_message>
<xml_diff>
--- a/Raw_qPCR.xlsx
+++ b/Raw_qPCR.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/Manuscripts/DBM_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDB12D3C-974E-45C6-A2EE-2FF3B32E095A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{CDB12D3C-974E-45C6-A2EE-2FF3B32E095A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34E54E35-2038-483A-A7B4-768B018A4358}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{13AE8149-C31B-407F-848D-7D619BD66D50}"/>
+    <workbookView xWindow="28680" yWindow="-4965" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{13AE8149-C31B-407F-848D-7D619BD66D50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
   <si>
     <t>Off Tet</t>
   </si>
@@ -49,12 +50,18 @@
   <si>
     <t>3DPE</t>
   </si>
+  <si>
+    <t>life_stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative_quantification_values </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +72,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,12 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,9 +421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42608EA7-3E87-452E-AB23-1FA6F8238990}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -543,6 +559,170 @@
         <v>-0.15490200000000001</v>
       </c>
     </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-0.85387199999999996</v>
+      </c>
+      <c r="C10">
+        <f>10^B10</f>
+        <v>0.13999998849869541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-0.95860730000000005</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C22" si="0">10^B11</f>
+        <v>0.11000000375918953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-0.82390870000000005</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.15000001414166733</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-0.42021639999999999</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.38000000296023134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.22914799999999999</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.58999998418385391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-0.34678750000000003</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.44999998572649469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-0.42021639999999999</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.38000000296023134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-1.0969100000000001</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>8.0000002396172554E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-6.5501500000000004E-2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.86000009654862275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.43296929000000001</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>2.7099999945437037</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-0.22184870000000001</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.60000006854753341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.30103000000000002</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2.0000000199681049</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-0.15490200000000001</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.69999993550464101</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
@@ -551,5 +731,133 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93520DB-F96D-4576-A928-B1FE885EA7B7}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.13999998849869541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.11000000375918953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.15000001414166733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.38000000296023134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.58999998418385391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.44999998572649469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.38000000296023134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>8.0000002396172554E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>0.86000009654862275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2.7099999945437037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>0.60000006854753341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2.0000000199681049</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>0.69999993550464101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>